<commit_message>
Multiple updates and changes. CSV done, DATA in progress.
All .csv files are being generated correctly, I believe I'm accounting for all data.

Combined CPU & SIM into DATA as I need to generate all *Info tables and inst_id's before
writing any configurations. Almost done parsing csv data into usable dicts.

Have not moved to History yet, that will come next.
</commit_message>
<xml_diff>
--- a/OCSInstrumentInventory_JK.xlsx
+++ b/OCSInstrumentInventory_JK.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9480" yWindow="460" windowWidth="31880" windowHeight="19760" tabRatio="500"/>
+    <workbookView xWindow="6520" yWindow="460" windowWidth="31880" windowHeight="19760" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="In Service" sheetId="1" r:id="rId1"/>
@@ -672,7 +672,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2312" uniqueCount="839">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2332" uniqueCount="843">
   <si>
     <t>New 6/14.</t>
     <phoneticPr fontId="7" type="noConversion"/>
@@ -3816,6 +3816,18 @@
   </si>
   <si>
     <t>Masked</t>
+  </si>
+  <si>
+    <t>A1971</t>
+  </si>
+  <si>
+    <t>A1972</t>
+  </si>
+  <si>
+    <t>A1973</t>
+  </si>
+  <si>
+    <t>A1974</t>
   </si>
 </sst>
 </file>
@@ -5019,7 +5031,7 @@
   </sheetPr>
   <dimension ref="A1:M204"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A94" sqref="A94:XFD94"/>
     </sheetView>
@@ -21296,10 +21308,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -21720,58 +21732,130 @@
     </row>
     <row r="15" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>832</v>
-      </c>
-      <c r="B15" s="46">
-        <v>8821</v>
+        <v>628</v>
+      </c>
+      <c r="B15" s="46" t="s">
+        <v>839</v>
       </c>
       <c r="C15" t="s">
         <v>84</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>755</v>
-      </c>
-      <c r="E15" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>618</v>
       </c>
-      <c r="J15" s="43">
-        <v>41852</v>
-      </c>
+      <c r="J15" s="43"/>
     </row>
     <row r="16" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
+        <v>628</v>
+      </c>
+      <c r="B16" s="46" t="s">
+        <v>840</v>
+      </c>
+      <c r="C16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>618</v>
+      </c>
+      <c r="J16" s="43"/>
+    </row>
+    <row r="17" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>628</v>
+      </c>
+      <c r="B17" s="46" t="s">
+        <v>841</v>
+      </c>
+      <c r="C17" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>618</v>
+      </c>
+      <c r="J17" s="43"/>
+    </row>
+    <row r="18" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>628</v>
+      </c>
+      <c r="B18" s="46" t="s">
+        <v>842</v>
+      </c>
+      <c r="C18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>618</v>
+      </c>
+      <c r="J18" s="43"/>
+    </row>
+    <row r="19" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
         <v>832</v>
       </c>
-      <c r="B16">
+      <c r="B19" s="46">
+        <v>8821</v>
+      </c>
+      <c r="C19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="34" t="s">
+        <v>755</v>
+      </c>
+      <c r="E19" t="s">
+        <v>84</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>618</v>
+      </c>
+      <c r="J19" s="43">
+        <v>41852</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>832</v>
+      </c>
+      <c r="B20">
         <v>2142</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C20" t="s">
         <v>837</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E20" t="s">
         <v>836</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G20" s="5" t="s">
         <v>835</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" t="s">
+    <row r="21" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
         <v>832</v>
       </c>
-      <c r="B17">
+      <c r="B21">
         <v>2143</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C21" t="s">
         <v>837</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E21" t="s">
         <v>836</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G21" s="5" t="s">
         <v>835</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added in SIM location inserts to initial build Additionally cleaned up the code in various files. Removed the building of the test database in Makefile.
</commit_message>
<xml_diff>
--- a/OCSInstrumentInventory_JK.xlsx
+++ b/OCSInstrumentInventory_JK.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28908"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Projects/OCS/Inventory/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9DEB5FA-E525-2B46-9AF5-0F8EEA193481}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6520" yWindow="460" windowWidth="31880" windowHeight="19760" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="4360" yWindow="460" windowWidth="31880" windowHeight="19760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="In Service" sheetId="1" r:id="rId1"/>
@@ -19,11 +20,12 @@
     <sheet name="TPOS-Saildrone" sheetId="8" r:id="rId5"/>
     <sheet name="EPIC" sheetId="5" r:id="rId6"/>
     <sheet name="EPIC2" sheetId="4" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="10" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'In Service'!$A$1:$M$204</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'In Service'!$A$1:$M$205</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -36,12 +38,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Jennifer Keene</author>
   </authors>
   <commentList>
-    <comment ref="E6" authorId="0">
+    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
       <text>
         <r>
           <rPr>
@@ -63,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H11" authorId="0">
+    <comment ref="H11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000002000000}">
       <text>
         <r>
           <rPr>
@@ -85,7 +87,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E13" authorId="0">
+    <comment ref="E13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000003000000}">
       <text>
         <r>
           <rPr>
@@ -107,7 +109,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E14" authorId="0">
+    <comment ref="E14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000004000000}">
       <text>
         <r>
           <rPr>
@@ -129,7 +131,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F14" authorId="0">
+    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000005000000}">
       <text>
         <r>
           <rPr>
@@ -151,7 +153,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G14" authorId="0">
+    <comment ref="G14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000006000000}">
       <text>
         <r>
           <rPr>
@@ -173,7 +175,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E15" authorId="0">
+    <comment ref="E15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000007000000}">
       <text>
         <r>
           <rPr>
@@ -195,7 +197,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F15" authorId="0">
+    <comment ref="F15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000008000000}">
       <text>
         <r>
           <rPr>
@@ -217,7 +219,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H15" authorId="0">
+    <comment ref="H15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000009000000}">
       <text>
         <r>
           <rPr>
@@ -239,7 +241,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E16" authorId="0">
+    <comment ref="E16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -261,7 +263,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E17" authorId="0">
+    <comment ref="E17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -283,7 +285,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G17" authorId="0">
+    <comment ref="G17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -305,7 +307,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E21" authorId="0">
+    <comment ref="E21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -327,7 +329,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G21" authorId="0">
+    <comment ref="G21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -354,12 +356,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Jennifer Keene</author>
   </authors>
   <commentList>
-    <comment ref="D6" authorId="0">
+    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
       <text>
         <r>
           <rPr>
@@ -381,7 +383,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G11" authorId="0">
+    <comment ref="G11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000002000000}">
       <text>
         <r>
           <rPr>
@@ -403,7 +405,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D13" authorId="0">
+    <comment ref="D13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000003000000}">
       <text>
         <r>
           <rPr>
@@ -425,7 +427,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D14" authorId="0">
+    <comment ref="D14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000004000000}">
       <text>
         <r>
           <rPr>
@@ -447,7 +449,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E14" authorId="0">
+    <comment ref="E14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000005000000}">
       <text>
         <r>
           <rPr>
@@ -469,7 +471,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F14" authorId="0">
+    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000006000000}">
       <text>
         <r>
           <rPr>
@@ -491,7 +493,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D15" authorId="0">
+    <comment ref="D15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000007000000}">
       <text>
         <r>
           <rPr>
@@ -513,7 +515,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E15" authorId="0">
+    <comment ref="E15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000008000000}">
       <text>
         <r>
           <rPr>
@@ -535,7 +537,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G15" authorId="0">
+    <comment ref="G15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000009000000}">
       <text>
         <r>
           <rPr>
@@ -557,7 +559,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D16" authorId="0">
+    <comment ref="D16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -579,7 +581,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D17" authorId="0">
+    <comment ref="D17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -601,7 +603,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F17" authorId="0">
+    <comment ref="F17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -623,7 +625,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D21" authorId="0">
+    <comment ref="D21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -645,7 +647,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F21" authorId="0">
+    <comment ref="F21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -672,7 +674,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2332" uniqueCount="843">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2353" uniqueCount="857">
   <si>
     <t>New 6/14.</t>
     <phoneticPr fontId="7" type="noConversion"/>
@@ -3829,11 +3831,53 @@
   <si>
     <t>A1974</t>
   </si>
+  <si>
+    <t>Damaged beyond repair.  Replaced under warranty.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OCS Lab - </t>
+  </si>
+  <si>
+    <t>OCS Lab - Calibrated</t>
+  </si>
+  <si>
+    <t>OCS Lab - Needs Cal</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>OCS Lab</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>PAPA</t>
+  </si>
+  <si>
+    <t>SEABIRD</t>
+  </si>
+  <si>
+    <t>In for Cal/Repair</t>
+  </si>
+  <si>
+    <t>Digital S/N reads 1913</t>
+  </si>
+  <si>
+    <t>Digital S/N reads 1914</t>
+  </si>
+  <si>
+    <t>Digital S/N reads 1915</t>
+  </si>
+  <si>
+    <t>Digital S/N reads 1916</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -4706,6 +4750,17 @@
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B9" totalsRowShown="0">
+  <autoFilter ref="A1:B9" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Status"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Location"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5025,15 +5080,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M204"/>
+  <dimension ref="A1:M205"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A94" sqref="A94:XFD94"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.6640625" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5043,11 +5098,11 @@
     <col min="3" max="3" width="12.6640625" style="46" customWidth="1"/>
     <col min="4" max="4" width="0.1640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="11.1640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="7.83203125" customWidth="1"/>
-    <col min="7" max="7" width="6.1640625" style="38" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="7.1640625" style="38" customWidth="1"/>
     <col min="8" max="8" width="14.5" customWidth="1"/>
     <col min="9" max="9" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.1640625" customWidth="1"/>
     <col min="11" max="11" width="41.33203125" customWidth="1"/>
     <col min="12" max="12" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -8439,13 +8494,13 @@
     </row>
     <row r="132" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A132" t="s">
-        <v>82</v>
+        <v>451</v>
       </c>
       <c r="B132" s="36" t="s">
-        <v>87</v>
+        <v>479</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>196</v>
+        <v>480</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>563</v>
@@ -8460,18 +8515,21 @@
         <v>634</v>
       </c>
       <c r="J132">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="K132" s="5" t="s">
-        <v>86</v>
+        <v>482</v>
+      </c>
+      <c r="L132" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="133" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A133" t="s">
         <v>451</v>
       </c>
-      <c r="B133" s="36" t="s">
-        <v>479</v>
+      <c r="B133" s="46">
+        <v>20087</v>
       </c>
       <c r="D133" s="2" t="s">
         <v>480</v>
@@ -8480,89 +8538,69 @@
         <v>563</v>
       </c>
       <c r="F133" t="s">
-        <v>518</v>
+        <v>84</v>
       </c>
       <c r="G133" s="38" t="s">
-        <v>584</v>
-      </c>
-      <c r="H133" s="7" t="s">
-        <v>634</v>
-      </c>
-      <c r="J133">
-        <v>14</v>
-      </c>
-      <c r="K133" s="5" t="s">
-        <v>482</v>
-      </c>
-      <c r="L133" t="s">
-        <v>537</v>
-      </c>
+        <v>848</v>
+      </c>
+      <c r="H133" s="7"/>
+      <c r="K133" s="5"/>
     </row>
     <row r="134" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A134" t="s">
-        <v>173</v>
-      </c>
-      <c r="B134" s="36" t="s">
-        <v>325</v>
+        <v>451</v>
+      </c>
+      <c r="B134" s="46">
+        <v>20433</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>311</v>
+        <v>480</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F134" t="s">
-        <v>541</v>
+        <v>844</v>
       </c>
       <c r="G134" s="38" t="s">
-        <v>85</v>
-      </c>
-      <c r="H134" s="7" t="s">
-        <v>500</v>
-      </c>
-      <c r="I134" t="s">
-        <v>771</v>
-      </c>
-      <c r="J134">
-        <v>525</v>
-      </c>
-      <c r="K134" s="5" t="s">
-        <v>347</v>
-      </c>
-      <c r="L134" t="s">
-        <v>658</v>
-      </c>
+        <v>848</v>
+      </c>
+      <c r="H134" s="7"/>
+      <c r="K134" s="5"/>
     </row>
     <row r="135" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A135" t="s">
         <v>173</v>
       </c>
       <c r="B135" s="36" t="s">
-        <v>343</v>
+        <v>325</v>
       </c>
       <c r="D135" s="2" t="s">
         <v>311</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="F135" t="s">
-        <v>518</v>
+        <v>541</v>
       </c>
       <c r="G135" s="38" t="s">
-        <v>553</v>
-      </c>
-      <c r="H135" t="s">
-        <v>638</v>
+        <v>85</v>
+      </c>
+      <c r="H135" s="7" t="s">
+        <v>500</v>
+      </c>
+      <c r="I135" t="s">
+        <v>771</v>
       </c>
       <c r="J135">
-        <v>75</v>
+        <v>525</v>
       </c>
       <c r="K135" s="5" t="s">
-        <v>450</v>
+        <v>347</v>
       </c>
       <c r="L135" t="s">
-        <v>644</v>
+        <v>658</v>
       </c>
     </row>
     <row r="136" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -8570,13 +8608,13 @@
         <v>173</v>
       </c>
       <c r="B136" s="36" t="s">
-        <v>411</v>
+        <v>343</v>
       </c>
       <c r="D136" s="2" t="s">
         <v>311</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F136" t="s">
         <v>518</v>
@@ -8588,13 +8626,13 @@
         <v>638</v>
       </c>
       <c r="J136">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="K136" s="5" t="s">
-        <v>488</v>
+        <v>450</v>
       </c>
       <c r="L136" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="137" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -8602,7 +8640,7 @@
         <v>173</v>
       </c>
       <c r="B137" s="36" t="s">
-        <v>384</v>
+        <v>411</v>
       </c>
       <c r="D137" s="2" t="s">
         <v>311</v>
@@ -8620,13 +8658,13 @@
         <v>638</v>
       </c>
       <c r="J137">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="K137" s="5" t="s">
         <v>488</v>
       </c>
       <c r="L137" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="138" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -8634,7 +8672,7 @@
         <v>173</v>
       </c>
       <c r="B138" s="36" t="s">
-        <v>118</v>
+        <v>384</v>
       </c>
       <c r="D138" s="2" t="s">
         <v>311</v>
@@ -8652,13 +8690,13 @@
         <v>638</v>
       </c>
       <c r="J138">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="K138" s="5" t="s">
         <v>488</v>
       </c>
       <c r="L138" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="139" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -8666,7 +8704,7 @@
         <v>173</v>
       </c>
       <c r="B139" s="36" t="s">
-        <v>18</v>
+        <v>118</v>
       </c>
       <c r="D139" s="2" t="s">
         <v>311</v>
@@ -8684,13 +8722,13 @@
         <v>638</v>
       </c>
       <c r="J139">
-        <v>175</v>
+        <v>150</v>
       </c>
       <c r="K139" s="5" t="s">
         <v>488</v>
       </c>
       <c r="L139" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="140" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -8698,13 +8736,13 @@
         <v>173</v>
       </c>
       <c r="B140" s="36" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D140" s="2" t="s">
         <v>311</v>
       </c>
       <c r="E140" s="2" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="F140" t="s">
         <v>518</v>
@@ -8716,13 +8754,13 @@
         <v>638</v>
       </c>
       <c r="J140">
-        <v>225</v>
+        <v>175</v>
       </c>
       <c r="K140" s="5" t="s">
-        <v>450</v>
+        <v>488</v>
       </c>
       <c r="L140" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="141" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -8730,13 +8768,13 @@
         <v>173</v>
       </c>
       <c r="B141" s="36" t="s">
-        <v>286</v>
+        <v>26</v>
       </c>
       <c r="D141" s="2" t="s">
         <v>311</v>
       </c>
       <c r="E141" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F141" t="s">
         <v>518</v>
@@ -8748,13 +8786,13 @@
         <v>638</v>
       </c>
       <c r="J141">
-        <v>275</v>
+        <v>225</v>
       </c>
       <c r="K141" s="5" t="s">
-        <v>488</v>
+        <v>450</v>
       </c>
       <c r="L141" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="142" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -8762,7 +8800,7 @@
         <v>173</v>
       </c>
       <c r="B142" s="36" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D142" s="2" t="s">
         <v>311</v>
@@ -8780,13 +8818,13 @@
         <v>638</v>
       </c>
       <c r="J142">
-        <v>325</v>
+        <v>275</v>
       </c>
       <c r="K142" s="5" t="s">
-        <v>382</v>
+        <v>488</v>
       </c>
       <c r="L142" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="143" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -8794,7 +8832,7 @@
         <v>173</v>
       </c>
       <c r="B143" s="36" t="s">
-        <v>170</v>
+        <v>287</v>
       </c>
       <c r="D143" s="2" t="s">
         <v>311</v>
@@ -8812,61 +8850,57 @@
         <v>638</v>
       </c>
       <c r="J143">
-        <v>525</v>
+        <v>325</v>
       </c>
       <c r="K143" s="5" t="s">
         <v>382</v>
       </c>
       <c r="L143" t="s">
-        <v>652</v>
-      </c>
-      <c r="M143" s="7"/>
+        <v>651</v>
+      </c>
     </row>
     <row r="144" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A144" t="s">
         <v>173</v>
       </c>
       <c r="B144" s="36" t="s">
-        <v>280</v>
+        <v>170</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>195</v>
+        <v>311</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>564</v>
       </c>
       <c r="F144" t="s">
-        <v>541</v>
+        <v>518</v>
       </c>
       <c r="G144" s="38" t="s">
-        <v>85</v>
+        <v>553</v>
       </c>
       <c r="H144" t="s">
-        <v>555</v>
-      </c>
-      <c r="I144" t="s">
-        <v>760</v>
+        <v>638</v>
       </c>
       <c r="J144">
-        <v>15</v>
-      </c>
-      <c r="K144" t="s">
-        <v>158</v>
+        <v>525</v>
+      </c>
+      <c r="K144" s="5" t="s">
+        <v>382</v>
       </c>
       <c r="L144" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="145" spans="1:13" s="7" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+        <v>652</v>
+      </c>
+      <c r="M144" s="7"/>
+    </row>
+    <row r="145" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A145" t="s">
         <v>173</v>
       </c>
       <c r="B145" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="C145" s="46"/>
+        <v>280</v>
+      </c>
       <c r="D145" s="2" t="s">
-        <v>311</v>
+        <v>195</v>
       </c>
       <c r="E145" s="2" t="s">
         <v>564</v>
@@ -8877,30 +8911,30 @@
       <c r="G145" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="H145" s="7" t="s">
+      <c r="H145" t="s">
         <v>555</v>
       </c>
       <c r="I145" t="s">
         <v>760</v>
       </c>
       <c r="J145">
-        <v>25</v>
-      </c>
-      <c r="K145" s="5" t="s">
-        <v>237</v>
+        <v>15</v>
+      </c>
+      <c r="K145" t="s">
+        <v>158</v>
       </c>
       <c r="L145" t="s">
-        <v>660</v>
-      </c>
-      <c r="M145"/>
-    </row>
-    <row r="146" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" s="7" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A146" t="s">
         <v>173</v>
       </c>
       <c r="B146" s="36" t="s">
-        <v>394</v>
-      </c>
+        <v>359</v>
+      </c>
+      <c r="C146" s="46"/>
       <c r="D146" s="2" t="s">
         <v>311</v>
       </c>
@@ -8920,24 +8954,25 @@
         <v>760</v>
       </c>
       <c r="J146">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="K146" s="5" t="s">
-        <v>317</v>
+        <v>237</v>
       </c>
       <c r="L146" t="s">
-        <v>661</v>
-      </c>
+        <v>660</v>
+      </c>
+      <c r="M146"/>
     </row>
     <row r="147" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A147" t="s">
         <v>173</v>
       </c>
       <c r="B147" s="36" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>169</v>
+        <v>311</v>
       </c>
       <c r="E147" s="2" t="s">
         <v>564</v>
@@ -8955,13 +8990,13 @@
         <v>760</v>
       </c>
       <c r="J147">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="K147" s="5" t="s">
-        <v>255</v>
+        <v>317</v>
       </c>
       <c r="L147" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="148" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -8969,7 +9004,7 @@
         <v>173</v>
       </c>
       <c r="B148" s="36" t="s">
-        <v>266</v>
+        <v>395</v>
       </c>
       <c r="D148" s="2" t="s">
         <v>169</v>
@@ -8990,13 +9025,13 @@
         <v>760</v>
       </c>
       <c r="J148">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="K148" s="5" t="s">
-        <v>368</v>
+        <v>255</v>
       </c>
       <c r="L148" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="149" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -9004,7 +9039,7 @@
         <v>173</v>
       </c>
       <c r="B149" s="36" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="D149" s="2" t="s">
         <v>169</v>
@@ -9025,13 +9060,13 @@
         <v>760</v>
       </c>
       <c r="J149">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="K149" s="5" t="s">
-        <v>237</v>
+        <v>368</v>
       </c>
       <c r="L149" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="150" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -9039,7 +9074,7 @@
         <v>173</v>
       </c>
       <c r="B150" s="36" t="s">
-        <v>164</v>
+        <v>273</v>
       </c>
       <c r="D150" s="2" t="s">
         <v>169</v>
@@ -9060,13 +9095,13 @@
         <v>760</v>
       </c>
       <c r="J150">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="K150" s="5" t="s">
-        <v>426</v>
+        <v>237</v>
       </c>
       <c r="L150" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="151" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -9074,7 +9109,7 @@
         <v>173</v>
       </c>
       <c r="B151" s="36" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D151" s="2" t="s">
         <v>169</v>
@@ -9083,30 +9118,33 @@
         <v>564</v>
       </c>
       <c r="F151" t="s">
-        <v>518</v>
+        <v>541</v>
       </c>
       <c r="G151" s="38" t="s">
-        <v>553</v>
-      </c>
-      <c r="H151" t="s">
-        <v>638</v>
+        <v>85</v>
+      </c>
+      <c r="H151" s="7" t="s">
+        <v>555</v>
+      </c>
+      <c r="I151" t="s">
+        <v>760</v>
       </c>
       <c r="J151">
-        <v>425</v>
+        <v>125</v>
       </c>
       <c r="K151" s="5" t="s">
-        <v>363</v>
+        <v>426</v>
       </c>
       <c r="L151" t="s">
-        <v>673</v>
+        <v>665</v>
       </c>
     </row>
     <row r="152" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A152" t="s">
         <v>173</v>
       </c>
-      <c r="B152" s="46" t="s">
-        <v>326</v>
+      <c r="B152" s="36" t="s">
+        <v>165</v>
       </c>
       <c r="D152" s="2" t="s">
         <v>169</v>
@@ -9115,33 +9153,30 @@
         <v>564</v>
       </c>
       <c r="F152" t="s">
-        <v>541</v>
+        <v>518</v>
       </c>
       <c r="G152" s="38" t="s">
-        <v>85</v>
-      </c>
-      <c r="H152" s="7" t="s">
-        <v>555</v>
-      </c>
-      <c r="I152" t="s">
-        <v>760</v>
+        <v>553</v>
+      </c>
+      <c r="H152" t="s">
+        <v>638</v>
       </c>
       <c r="J152">
-        <v>175</v>
+        <v>425</v>
       </c>
       <c r="K152" s="5" t="s">
-        <v>255</v>
+        <v>363</v>
       </c>
       <c r="L152" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="153" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A153" t="s">
         <v>173</v>
       </c>
-      <c r="B153" s="36" t="s">
-        <v>210</v>
+      <c r="B153" s="46" t="s">
+        <v>326</v>
       </c>
       <c r="D153" s="2" t="s">
         <v>169</v>
@@ -9162,13 +9197,13 @@
         <v>760</v>
       </c>
       <c r="J153">
-        <v>225</v>
+        <v>175</v>
       </c>
       <c r="K153" s="5" t="s">
-        <v>362</v>
+        <v>255</v>
       </c>
       <c r="L153" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="154" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -9176,7 +9211,7 @@
         <v>173</v>
       </c>
       <c r="B154" s="36" t="s">
-        <v>11</v>
+        <v>210</v>
       </c>
       <c r="D154" s="2" t="s">
         <v>169</v>
@@ -9197,13 +9232,13 @@
         <v>760</v>
       </c>
       <c r="J154">
-        <v>275</v>
+        <v>225</v>
       </c>
       <c r="K154" s="5" t="s">
-        <v>275</v>
+        <v>362</v>
       </c>
       <c r="L154" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="155" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -9211,7 +9246,7 @@
         <v>173</v>
       </c>
       <c r="B155" s="36" t="s">
-        <v>105</v>
+        <v>11</v>
       </c>
       <c r="D155" s="2" t="s">
         <v>169</v>
@@ -9232,13 +9267,13 @@
         <v>760</v>
       </c>
       <c r="J155">
-        <v>325</v>
+        <v>275</v>
       </c>
       <c r="K155" s="5" t="s">
-        <v>303</v>
+        <v>275</v>
       </c>
       <c r="L155" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="156" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -9246,7 +9281,7 @@
         <v>173</v>
       </c>
       <c r="B156" s="36" t="s">
-        <v>265</v>
+        <v>105</v>
       </c>
       <c r="D156" s="2" t="s">
         <v>169</v>
@@ -9255,25 +9290,25 @@
         <v>564</v>
       </c>
       <c r="F156" t="s">
-        <v>559</v>
+        <v>541</v>
       </c>
       <c r="G156" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="H156" t="s">
-        <v>637</v>
+      <c r="H156" s="7" t="s">
+        <v>555</v>
       </c>
       <c r="I156" t="s">
         <v>760</v>
       </c>
       <c r="J156">
-        <v>525</v>
+        <v>325</v>
       </c>
       <c r="K156" s="5" t="s">
-        <v>759</v>
+        <v>303</v>
       </c>
       <c r="L156" t="s">
-        <v>657</v>
+        <v>677</v>
       </c>
     </row>
     <row r="157" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -9281,31 +9316,34 @@
         <v>173</v>
       </c>
       <c r="B157" s="36" t="s">
-        <v>254</v>
+        <v>265</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>107</v>
+        <v>169</v>
       </c>
       <c r="E157" s="2" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="F157" t="s">
-        <v>541</v>
+        <v>559</v>
       </c>
       <c r="G157" s="38" t="s">
         <v>85</v>
       </c>
       <c r="H157" t="s">
-        <v>555</v>
+        <v>637</v>
       </c>
       <c r="I157" t="s">
         <v>760</v>
       </c>
       <c r="J157">
-        <v>150</v>
+        <v>525</v>
       </c>
       <c r="K157" s="5" t="s">
-        <v>342</v>
+        <v>759</v>
+      </c>
+      <c r="L157" t="s">
+        <v>657</v>
       </c>
     </row>
     <row r="158" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -9313,36 +9351,39 @@
         <v>173</v>
       </c>
       <c r="B158" s="36" t="s">
-        <v>88</v>
+        <v>254</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>196</v>
+        <v>107</v>
       </c>
       <c r="E158" s="2" t="s">
         <v>563</v>
       </c>
       <c r="F158" t="s">
-        <v>518</v>
+        <v>541</v>
       </c>
       <c r="G158" s="38" t="s">
-        <v>553</v>
+        <v>85</v>
       </c>
       <c r="H158" t="s">
-        <v>638</v>
+        <v>555</v>
+      </c>
+      <c r="I158" t="s">
+        <v>760</v>
       </c>
       <c r="J158">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="K158" s="5" t="s">
-        <v>86</v>
+        <v>342</v>
       </c>
     </row>
     <row r="159" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A159" t="s">
         <v>173</v>
       </c>
-      <c r="B159" s="36">
-        <v>16293</v>
+      <c r="B159" s="36" t="s">
+        <v>88</v>
       </c>
       <c r="D159" s="2" t="s">
         <v>196</v>
@@ -9351,52 +9392,51 @@
         <v>563</v>
       </c>
       <c r="F159" t="s">
-        <v>84</v>
+        <v>518</v>
       </c>
       <c r="G159" s="38" t="s">
-        <v>85</v>
-      </c>
-      <c r="H159" s="7" t="s">
-        <v>787</v>
+        <v>553</v>
+      </c>
+      <c r="H159" t="s">
+        <v>638</v>
       </c>
       <c r="J159">
-        <v>425</v>
+        <v>50</v>
       </c>
       <c r="K159" s="5" t="s">
-        <v>786</v>
-      </c>
-      <c r="L159" t="s">
-        <v>788</v>
+        <v>86</v>
       </c>
     </row>
     <row r="160" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A160" s="7" t="s">
-        <v>507</v>
-      </c>
-      <c r="B160" s="47" t="s">
-        <v>508</v>
-      </c>
-      <c r="C160" s="47"/>
+      <c r="A160" t="s">
+        <v>173</v>
+      </c>
+      <c r="B160" s="36">
+        <v>16293</v>
+      </c>
       <c r="D160" s="2" t="s">
-        <v>509</v>
+        <v>196</v>
       </c>
       <c r="E160" s="2" t="s">
         <v>563</v>
       </c>
       <c r="F160" t="s">
-        <v>518</v>
+        <v>84</v>
       </c>
       <c r="G160" s="38" t="s">
-        <v>584</v>
+        <v>85</v>
       </c>
       <c r="H160" s="7" t="s">
-        <v>634</v>
+        <v>787</v>
       </c>
       <c r="J160">
-        <v>4250</v>
+        <v>425</v>
       </c>
       <c r="K160" s="5" t="s">
-        <v>510</v>
+        <v>786</v>
+      </c>
+      <c r="L160" t="s">
+        <v>788</v>
       </c>
     </row>
     <row r="161" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -9404,7 +9444,7 @@
         <v>507</v>
       </c>
       <c r="B161" s="47" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="C161" s="47"/>
       <c r="D161" s="2" t="s">
@@ -9417,45 +9457,46 @@
         <v>518</v>
       </c>
       <c r="G161" s="38" t="s">
-        <v>553</v>
-      </c>
-      <c r="H161" t="s">
-        <v>638</v>
+        <v>584</v>
+      </c>
+      <c r="H161" s="7" t="s">
+        <v>634</v>
       </c>
       <c r="J161">
-        <v>5700</v>
+        <v>4250</v>
       </c>
       <c r="K161" s="5" t="s">
         <v>510</v>
       </c>
     </row>
     <row r="162" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A162" t="s">
-        <v>199</v>
-      </c>
-      <c r="B162" s="46" t="s">
-        <v>200</v>
-      </c>
+      <c r="A162" s="7" t="s">
+        <v>507</v>
+      </c>
+      <c r="B162" s="47" t="s">
+        <v>511</v>
+      </c>
+      <c r="C162" s="47"/>
       <c r="D162" s="2" t="s">
-        <v>201</v>
+        <v>509</v>
       </c>
       <c r="E162" s="2" t="s">
         <v>563</v>
       </c>
       <c r="F162" t="s">
-        <v>541</v>
+        <v>518</v>
       </c>
       <c r="G162" s="38" t="s">
-        <v>85</v>
-      </c>
-      <c r="H162" s="7" t="s">
-        <v>555</v>
+        <v>553</v>
+      </c>
+      <c r="H162" t="s">
+        <v>638</v>
       </c>
       <c r="J162">
         <v>5700</v>
       </c>
       <c r="K162" s="5" t="s">
-        <v>134</v>
+        <v>510</v>
       </c>
     </row>
     <row r="163" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -9463,10 +9504,10 @@
         <v>199</v>
       </c>
       <c r="B163" s="46" t="s">
-        <v>89</v>
+        <v>200</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="E163" s="2" t="s">
         <v>563</v>
@@ -9477,75 +9518,75 @@
       <c r="G163" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="H163" t="s">
-        <v>455</v>
-      </c>
-      <c r="I163" t="s">
-        <v>768</v>
+      <c r="H163" s="7" t="s">
+        <v>555</v>
       </c>
       <c r="J163">
-        <v>4250</v>
+        <v>5700</v>
       </c>
       <c r="K163" s="5" t="s">
-        <v>39</v>
+        <v>134</v>
       </c>
     </row>
     <row r="164" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A164" t="s">
-        <v>328</v>
-      </c>
-      <c r="B164" s="36" t="s">
-        <v>162</v>
+        <v>199</v>
+      </c>
+      <c r="B164" s="46" t="s">
+        <v>89</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>169</v>
+        <v>195</v>
       </c>
       <c r="E164" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F164" t="s">
-        <v>518</v>
-      </c>
-      <c r="G164" s="34" t="s">
-        <v>553</v>
+        <v>541</v>
+      </c>
+      <c r="G164" s="38" t="s">
+        <v>85</v>
       </c>
       <c r="H164" t="s">
-        <v>639</v>
+        <v>455</v>
+      </c>
+      <c r="I164" t="s">
+        <v>768</v>
       </c>
       <c r="J164">
-        <v>1</v>
+        <v>4250</v>
       </c>
       <c r="K164" s="5" t="s">
-        <v>472</v>
+        <v>39</v>
       </c>
     </row>
     <row r="165" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A165" t="s">
-        <v>155</v>
+        <v>328</v>
       </c>
       <c r="B165" s="36" t="s">
-        <v>101</v>
+        <v>162</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>195</v>
+        <v>169</v>
       </c>
       <c r="E165" s="2" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="F165" t="s">
-        <v>502</v>
-      </c>
-      <c r="G165" s="38" t="s">
-        <v>2</v>
+        <v>518</v>
+      </c>
+      <c r="G165" s="34" t="s">
+        <v>553</v>
       </c>
       <c r="H165" t="s">
-        <v>424</v>
+        <v>639</v>
       </c>
       <c r="J165">
         <v>1</v>
       </c>
       <c r="K165" s="5" t="s">
-        <v>501</v>
+        <v>472</v>
       </c>
     </row>
     <row r="166" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -9553,34 +9594,28 @@
         <v>155</v>
       </c>
       <c r="B166" s="36" t="s">
-        <v>156</v>
+        <v>101</v>
       </c>
       <c r="D166" s="2" t="s">
         <v>195</v>
       </c>
       <c r="E166" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F166" t="s">
-        <v>541</v>
+        <v>502</v>
       </c>
       <c r="G166" s="38" t="s">
-        <v>85</v>
+        <v>2</v>
       </c>
       <c r="H166" t="s">
-        <v>555</v>
-      </c>
-      <c r="I166" t="s">
-        <v>771</v>
+        <v>424</v>
       </c>
       <c r="J166">
         <v>1</v>
       </c>
-      <c r="K166" t="s">
-        <v>141</v>
-      </c>
-      <c r="L166" t="s">
-        <v>687</v>
+      <c r="K166" s="5" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="167" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -9588,34 +9623,34 @@
         <v>155</v>
       </c>
       <c r="B167" s="36" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>65</v>
+        <v>195</v>
       </c>
       <c r="E167" s="2" t="s">
         <v>564</v>
       </c>
       <c r="F167" t="s">
-        <v>492</v>
+        <v>541</v>
       </c>
       <c r="G167" s="38" t="s">
-        <v>207</v>
+        <v>85</v>
       </c>
       <c r="H167" t="s">
-        <v>637</v>
+        <v>555</v>
       </c>
       <c r="I167" t="s">
-        <v>760</v>
+        <v>771</v>
       </c>
       <c r="J167">
         <v>1</v>
       </c>
-      <c r="K167" s="5" t="s">
-        <v>397</v>
+      <c r="K167" t="s">
+        <v>141</v>
       </c>
       <c r="L167" t="s">
-        <v>671</v>
+        <v>687</v>
       </c>
     </row>
     <row r="168" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -9623,31 +9658,34 @@
         <v>155</v>
       </c>
       <c r="B168" s="36" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>196</v>
+        <v>65</v>
       </c>
       <c r="E168" s="2" t="s">
         <v>564</v>
       </c>
       <c r="F168" t="s">
-        <v>518</v>
+        <v>492</v>
       </c>
       <c r="G168" s="38" t="s">
-        <v>584</v>
+        <v>207</v>
       </c>
       <c r="H168" t="s">
-        <v>635</v>
+        <v>637</v>
+      </c>
+      <c r="I168" t="s">
+        <v>760</v>
       </c>
       <c r="J168">
         <v>1</v>
       </c>
       <c r="K168" s="5" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="L168" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="169" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -9655,7 +9693,7 @@
         <v>155</v>
       </c>
       <c r="B169" s="36" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D169" s="2" t="s">
         <v>196</v>
@@ -9669,49 +9707,49 @@
       <c r="G169" s="38" t="s">
         <v>584</v>
       </c>
-      <c r="H169" s="7" t="s">
-        <v>634</v>
+      <c r="H169" t="s">
+        <v>635</v>
       </c>
       <c r="J169">
         <v>1</v>
       </c>
       <c r="K169" s="5" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="L169" t="s">
-        <v>656</v>
+        <v>672</v>
       </c>
     </row>
     <row r="170" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A170" t="s">
-        <v>428</v>
+        <v>155</v>
       </c>
       <c r="B170" s="36" t="s">
-        <v>429</v>
+        <v>150</v>
       </c>
       <c r="D170" s="2" t="s">
         <v>196</v>
       </c>
       <c r="E170" s="2" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="F170" t="s">
-        <v>541</v>
+        <v>518</v>
       </c>
       <c r="G170" s="38" t="s">
-        <v>85</v>
+        <v>584</v>
       </c>
       <c r="H170" s="7" t="s">
-        <v>557</v>
-      </c>
-      <c r="I170" t="s">
-        <v>770</v>
+        <v>634</v>
       </c>
       <c r="J170">
         <v>1</v>
       </c>
       <c r="K170" s="5" t="s">
-        <v>430</v>
+        <v>407</v>
+      </c>
+      <c r="L170" t="s">
+        <v>656</v>
       </c>
     </row>
     <row r="171" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -9719,7 +9757,7 @@
         <v>428</v>
       </c>
       <c r="B171" s="36" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D171" s="2" t="s">
         <v>196</v>
@@ -9734,10 +9772,10 @@
         <v>85</v>
       </c>
       <c r="H171" s="7" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="I171" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="J171">
         <v>1</v>
@@ -9751,7 +9789,7 @@
         <v>428</v>
       </c>
       <c r="B172" s="36" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D172" s="2" t="s">
         <v>196</v>
@@ -9760,13 +9798,16 @@
         <v>563</v>
       </c>
       <c r="F172" t="s">
-        <v>518</v>
+        <v>541</v>
       </c>
       <c r="G172" s="38" t="s">
-        <v>553</v>
-      </c>
-      <c r="H172" t="s">
-        <v>638</v>
+        <v>85</v>
+      </c>
+      <c r="H172" s="7" t="s">
+        <v>560</v>
+      </c>
+      <c r="I172" t="s">
+        <v>769</v>
       </c>
       <c r="J172">
         <v>1</v>
@@ -9780,7 +9821,7 @@
         <v>428</v>
       </c>
       <c r="B173" s="36" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D173" s="2" t="s">
         <v>196</v>
@@ -9789,16 +9830,13 @@
         <v>563</v>
       </c>
       <c r="F173" t="s">
-        <v>492</v>
+        <v>518</v>
       </c>
       <c r="G173" s="38" t="s">
-        <v>85</v>
-      </c>
-      <c r="H173" s="7" t="s">
-        <v>636</v>
-      </c>
-      <c r="I173" t="s">
-        <v>768</v>
+        <v>553</v>
+      </c>
+      <c r="H173" t="s">
+        <v>638</v>
       </c>
       <c r="J173">
         <v>1</v>
@@ -9809,10 +9847,10 @@
     </row>
     <row r="174" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A174" t="s">
-        <v>40</v>
+        <v>428</v>
       </c>
       <c r="B174" s="36" t="s">
-        <v>41</v>
+        <v>433</v>
       </c>
       <c r="D174" s="2" t="s">
         <v>196</v>
@@ -9821,159 +9859,165 @@
         <v>563</v>
       </c>
       <c r="F174" t="s">
-        <v>541</v>
+        <v>492</v>
       </c>
       <c r="G174" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="H174" t="s">
-        <v>558</v>
+      <c r="H174" s="7" t="s">
+        <v>636</v>
       </c>
       <c r="I174" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="J174">
         <v>1</v>
       </c>
       <c r="K174" s="5" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="175" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A175" t="s">
+        <v>40</v>
+      </c>
+      <c r="B175" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="D175" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E175" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="F175" t="s">
+        <v>541</v>
+      </c>
+      <c r="G175" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="H175" t="s">
+        <v>558</v>
+      </c>
+      <c r="I175" t="s">
+        <v>772</v>
+      </c>
+      <c r="J175">
+        <v>1</v>
+      </c>
+      <c r="K175" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="175" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A175" s="7" t="s">
+    <row r="176" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A176" s="7" t="s">
         <v>409</v>
       </c>
-      <c r="B175" s="47" t="s">
+      <c r="B176" s="47" t="s">
         <v>413</v>
       </c>
-      <c r="C175" s="47"/>
-      <c r="D175" s="8" t="s">
+      <c r="C176" s="47"/>
+      <c r="D176" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E175" s="8"/>
-      <c r="F175" t="s">
+      <c r="E176" s="8"/>
+      <c r="F176" t="s">
         <v>796</v>
       </c>
-      <c r="G175" s="38" t="s">
+      <c r="G176" s="38" t="s">
         <v>792</v>
       </c>
-      <c r="H175" s="7" t="s">
+      <c r="H176" s="7" t="s">
         <v>270</v>
       </c>
-      <c r="I175" s="7"/>
-      <c r="J175" s="7"/>
-      <c r="K175" s="5" t="s">
+      <c r="I176" s="7"/>
+      <c r="J176" s="7"/>
+      <c r="K176" s="5" t="s">
         <v>799</v>
-      </c>
-    </row>
-    <row r="176" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A176" t="s">
-        <v>409</v>
-      </c>
-      <c r="B176" s="36" t="s">
-        <v>414</v>
-      </c>
-      <c r="D176" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F176" t="s">
-        <v>541</v>
-      </c>
-      <c r="G176" s="38" t="s">
-        <v>85</v>
-      </c>
-      <c r="H176" s="7" t="s">
-        <v>555</v>
-      </c>
-      <c r="I176" t="s">
-        <v>760</v>
-      </c>
-      <c r="J176" s="7">
-        <v>20</v>
-      </c>
-      <c r="K176" s="5" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="177" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A177" t="s">
         <v>409</v>
       </c>
-      <c r="B177" s="46" t="s">
-        <v>415</v>
+      <c r="B177" s="36" t="s">
+        <v>414</v>
       </c>
       <c r="D177" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F177" t="s">
-        <v>604</v>
+        <v>541</v>
       </c>
       <c r="G177" s="38" t="s">
-        <v>495</v>
+        <v>85</v>
       </c>
       <c r="H177" s="7" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I177" t="s">
-        <v>797</v>
-      </c>
-      <c r="J177">
-        <v>40</v>
+        <v>760</v>
+      </c>
+      <c r="J177" s="7">
+        <v>20</v>
       </c>
       <c r="K177" s="5" t="s">
-        <v>798</v>
+        <v>304</v>
       </c>
     </row>
     <row r="178" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A178" t="s">
         <v>409</v>
       </c>
-      <c r="B178" s="36" t="s">
-        <v>185</v>
+      <c r="B178" s="46" t="s">
+        <v>415</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>196</v>
+        <v>65</v>
       </c>
       <c r="F178" t="s">
-        <v>703</v>
+        <v>604</v>
       </c>
       <c r="G178" s="38" t="s">
-        <v>85</v>
+        <v>495</v>
       </c>
       <c r="H178" s="7" t="s">
-        <v>497</v>
+        <v>556</v>
+      </c>
+      <c r="I178" t="s">
+        <v>797</v>
       </c>
       <c r="J178">
         <v>40</v>
       </c>
-      <c r="K178" s="42" t="s">
-        <v>800</v>
+      <c r="K178" s="5" t="s">
+        <v>798</v>
       </c>
     </row>
     <row r="179" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A179" t="s">
-        <v>186</v>
+        <v>409</v>
       </c>
       <c r="B179" s="36" t="s">
-        <v>61</v>
+        <v>185</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>355</v>
+        <v>196</v>
       </c>
       <c r="F179" t="s">
-        <v>518</v>
+        <v>703</v>
       </c>
       <c r="G179" s="38" t="s">
-        <v>553</v>
+        <v>85</v>
       </c>
       <c r="H179" s="7" t="s">
-        <v>638</v>
-      </c>
-      <c r="J179" s="7">
-        <v>20</v>
-      </c>
-      <c r="K179" s="5" t="s">
-        <v>392</v>
+        <v>497</v>
+      </c>
+      <c r="J179">
+        <v>40</v>
+      </c>
+      <c r="K179" s="42" t="s">
+        <v>800</v>
       </c>
     </row>
     <row r="180" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -9981,7 +10025,7 @@
         <v>186</v>
       </c>
       <c r="B180" s="36" t="s">
-        <v>356</v>
+        <v>61</v>
       </c>
       <c r="D180" s="2" t="s">
         <v>355</v>
@@ -9996,10 +10040,10 @@
         <v>638</v>
       </c>
       <c r="J180" s="7">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="K180" s="5" t="s">
-        <v>335</v>
+        <v>392</v>
       </c>
     </row>
     <row r="181" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -10007,57 +10051,54 @@
         <v>186</v>
       </c>
       <c r="B181" s="36" t="s">
-        <v>98</v>
+        <v>356</v>
       </c>
       <c r="D181" s="2" t="s">
         <v>355</v>
       </c>
       <c r="F181" t="s">
-        <v>541</v>
+        <v>518</v>
       </c>
       <c r="G181" s="38" t="s">
-        <v>85</v>
+        <v>553</v>
       </c>
       <c r="H181" s="7" t="s">
-        <v>555</v>
-      </c>
-      <c r="I181" t="s">
-        <v>760</v>
-      </c>
-      <c r="J181">
-        <v>375</v>
-      </c>
-      <c r="K181" s="32" t="s">
-        <v>259</v>
+        <v>638</v>
+      </c>
+      <c r="J181" s="7">
+        <v>40</v>
+      </c>
+      <c r="K181" s="5" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="182" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A182" t="s">
         <v>186</v>
       </c>
-      <c r="B182" s="46" t="s">
-        <v>272</v>
+      <c r="B182" s="36" t="s">
+        <v>98</v>
       </c>
       <c r="D182" s="2" t="s">
         <v>355</v>
       </c>
       <c r="F182" t="s">
-        <v>559</v>
-      </c>
-      <c r="G182" s="34" t="s">
+        <v>541</v>
+      </c>
+      <c r="G182" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="H182" t="s">
-        <v>637</v>
+      <c r="H182" s="7" t="s">
+        <v>555</v>
       </c>
       <c r="I182" t="s">
         <v>760</v>
       </c>
       <c r="J182">
-        <v>5</v>
-      </c>
-      <c r="K182" s="5" t="s">
-        <v>301</v>
+        <v>375</v>
+      </c>
+      <c r="K182" s="32" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="183" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -10065,28 +10106,28 @@
         <v>186</v>
       </c>
       <c r="B183" s="46" t="s">
-        <v>445</v>
+        <v>272</v>
       </c>
       <c r="D183" s="2" t="s">
         <v>355</v>
       </c>
       <c r="F183" t="s">
-        <v>518</v>
-      </c>
-      <c r="G183" s="38" t="s">
-        <v>553</v>
+        <v>559</v>
+      </c>
+      <c r="G183" s="34" t="s">
+        <v>85</v>
       </c>
       <c r="H183" t="s">
-        <v>638</v>
+        <v>637</v>
+      </c>
+      <c r="I183" t="s">
+        <v>760</v>
       </c>
       <c r="J183">
         <v>5</v>
       </c>
       <c r="K183" s="5" t="s">
-        <v>308</v>
-      </c>
-      <c r="L183" t="s">
-        <v>683</v>
+        <v>301</v>
       </c>
     </row>
     <row r="184" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -10094,31 +10135,28 @@
         <v>186</v>
       </c>
       <c r="B184" s="46" t="s">
-        <v>253</v>
+        <v>445</v>
       </c>
       <c r="D184" s="2" t="s">
         <v>355</v>
       </c>
       <c r="F184" t="s">
-        <v>541</v>
+        <v>518</v>
       </c>
       <c r="G184" s="38" t="s">
-        <v>85</v>
-      </c>
-      <c r="H184" s="7" t="s">
-        <v>555</v>
-      </c>
-      <c r="I184" t="s">
-        <v>760</v>
+        <v>553</v>
+      </c>
+      <c r="H184" t="s">
+        <v>638</v>
       </c>
       <c r="J184">
-        <v>475</v>
-      </c>
-      <c r="K184" t="s">
-        <v>158</v>
+        <v>5</v>
+      </c>
+      <c r="K184" s="5" t="s">
+        <v>308</v>
       </c>
       <c r="L184" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="185" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -10126,51 +10164,57 @@
         <v>186</v>
       </c>
       <c r="B185" s="46" t="s">
-        <v>438</v>
+        <v>253</v>
       </c>
       <c r="D185" s="2" t="s">
         <v>355</v>
       </c>
       <c r="F185" t="s">
-        <v>518</v>
+        <v>541</v>
       </c>
       <c r="G185" s="38" t="s">
-        <v>553</v>
-      </c>
-      <c r="H185" t="s">
-        <v>638</v>
+        <v>85</v>
+      </c>
+      <c r="H185" s="7" t="s">
+        <v>555</v>
+      </c>
+      <c r="I185" t="s">
+        <v>760</v>
       </c>
       <c r="J185">
-        <v>375</v>
+        <v>475</v>
+      </c>
+      <c r="K185" t="s">
+        <v>158</v>
       </c>
       <c r="L185" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
     </row>
     <row r="186" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A186" t="s">
         <v>186</v>
       </c>
-      <c r="B186" s="36" t="s">
-        <v>94</v>
+      <c r="B186" s="46" t="s">
+        <v>438</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>169</v>
+        <v>355</v>
       </c>
       <c r="F186" t="s">
         <v>518</v>
       </c>
       <c r="G186" s="38" t="s">
-        <v>584</v>
+        <v>553</v>
       </c>
       <c r="H186" t="s">
-        <v>634</v>
+        <v>638</v>
       </c>
       <c r="J186">
-        <v>5</v>
+        <v>375</v>
       </c>
       <c r="L186" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="187" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -10178,28 +10222,25 @@
         <v>186</v>
       </c>
       <c r="B187" s="36" t="s">
-        <v>312</v>
+        <v>94</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>355</v>
+        <v>169</v>
       </c>
       <c r="F187" t="s">
-        <v>541</v>
+        <v>518</v>
       </c>
       <c r="G187" s="38" t="s">
-        <v>85</v>
+        <v>584</v>
       </c>
       <c r="H187" t="s">
-        <v>555</v>
-      </c>
-      <c r="I187" t="s">
-        <v>760</v>
+        <v>634</v>
       </c>
       <c r="J187">
-        <v>40</v>
-      </c>
-      <c r="K187" t="s">
-        <v>393</v>
+        <v>5</v>
+      </c>
+      <c r="L187" t="s">
+        <v>686</v>
       </c>
     </row>
     <row r="188" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -10207,26 +10248,28 @@
         <v>186</v>
       </c>
       <c r="B188" s="36" t="s">
-        <v>350</v>
+        <v>312</v>
       </c>
       <c r="D188" s="2" t="s">
         <v>355</v>
       </c>
       <c r="F188" t="s">
-        <v>703</v>
+        <v>541</v>
       </c>
       <c r="G188" s="38" t="s">
         <v>85</v>
       </c>
       <c r="H188" t="s">
-        <v>452</v>
-      </c>
-      <c r="I188" s="7"/>
+        <v>555</v>
+      </c>
+      <c r="I188" t="s">
+        <v>760</v>
+      </c>
       <c r="J188">
-        <v>300</v>
-      </c>
-      <c r="K188" s="5" t="s">
-        <v>738</v>
+        <v>40</v>
+      </c>
+      <c r="K188" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="189" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -10234,25 +10277,26 @@
         <v>186</v>
       </c>
       <c r="B189" s="36" t="s">
-        <v>74</v>
+        <v>350</v>
       </c>
       <c r="D189" s="2" t="s">
-        <v>169</v>
+        <v>355</v>
       </c>
       <c r="F189" t="s">
-        <v>518</v>
+        <v>703</v>
       </c>
       <c r="G189" s="38" t="s">
-        <v>553</v>
+        <v>85</v>
       </c>
       <c r="H189" t="s">
-        <v>638</v>
-      </c>
+        <v>452</v>
+      </c>
+      <c r="I189" s="7"/>
       <c r="J189">
-        <v>475</v>
+        <v>300</v>
       </c>
       <c r="K189" s="5" t="s">
-        <v>382</v>
+        <v>738</v>
       </c>
     </row>
     <row r="190" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -10260,25 +10304,22 @@
         <v>186</v>
       </c>
       <c r="B190" s="36" t="s">
-        <v>327</v>
+        <v>74</v>
       </c>
       <c r="D190" s="2" t="s">
-        <v>355</v>
+        <v>169</v>
       </c>
       <c r="F190" t="s">
-        <v>541</v>
+        <v>518</v>
       </c>
       <c r="G190" s="38" t="s">
-        <v>85</v>
-      </c>
-      <c r="H190" s="7" t="s">
-        <v>558</v>
-      </c>
-      <c r="I190" t="s">
-        <v>772</v>
+        <v>553</v>
+      </c>
+      <c r="H190" t="s">
+        <v>638</v>
       </c>
       <c r="J190">
-        <v>5</v>
+        <v>475</v>
       </c>
       <c r="K190" s="5" t="s">
         <v>382</v>
@@ -10288,8 +10329,8 @@
       <c r="A191" t="s">
         <v>186</v>
       </c>
-      <c r="B191" s="46" t="s">
-        <v>252</v>
+      <c r="B191" s="36" t="s">
+        <v>327</v>
       </c>
       <c r="D191" s="2" t="s">
         <v>355</v>
@@ -10301,67 +10342,70 @@
         <v>85</v>
       </c>
       <c r="H191" s="7" t="s">
-        <v>500</v>
+        <v>558</v>
       </c>
       <c r="I191" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="J191">
         <v>5</v>
       </c>
-      <c r="K191" s="5"/>
+      <c r="K191" s="5" t="s">
+        <v>382</v>
+      </c>
     </row>
     <row r="192" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A192" s="7" t="s">
+      <c r="A192" t="s">
         <v>186</v>
       </c>
-      <c r="B192" s="47" t="s">
-        <v>213</v>
-      </c>
-      <c r="C192" s="47"/>
+      <c r="B192" s="46" t="s">
+        <v>252</v>
+      </c>
       <c r="D192" s="2" t="s">
         <v>355</v>
       </c>
       <c r="F192" t="s">
-        <v>559</v>
+        <v>541</v>
       </c>
       <c r="G192" s="38" t="s">
         <v>85</v>
       </c>
       <c r="H192" s="7" t="s">
-        <v>636</v>
+        <v>500</v>
       </c>
       <c r="I192" t="s">
-        <v>768</v>
+        <v>771</v>
       </c>
       <c r="J192">
         <v>5</v>
       </c>
-      <c r="K192" s="5" t="s">
-        <v>407</v>
-      </c>
+      <c r="K192" s="5"/>
     </row>
     <row r="193" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A193" t="s">
+      <c r="A193" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="B193" s="36" t="s">
-        <v>143</v>
-      </c>
+      <c r="B193" s="47" t="s">
+        <v>213</v>
+      </c>
+      <c r="C193" s="47"/>
       <c r="D193" s="2" t="s">
         <v>355</v>
       </c>
       <c r="F193" t="s">
-        <v>518</v>
+        <v>559</v>
       </c>
       <c r="G193" s="38" t="s">
-        <v>584</v>
+        <v>85</v>
       </c>
       <c r="H193" s="7" t="s">
-        <v>634</v>
+        <v>636</v>
+      </c>
+      <c r="I193" t="s">
+        <v>768</v>
       </c>
       <c r="J193">
-        <v>175</v>
+        <v>5</v>
       </c>
       <c r="K193" s="5" t="s">
         <v>407</v>
@@ -10372,7 +10416,7 @@
         <v>186</v>
       </c>
       <c r="B194" s="36" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D194" s="2" t="s">
         <v>355</v>
@@ -10387,7 +10431,7 @@
         <v>634</v>
       </c>
       <c r="J194">
-        <v>300</v>
+        <v>175</v>
       </c>
       <c r="K194" s="5" t="s">
         <v>407</v>
@@ -10398,28 +10442,25 @@
         <v>186</v>
       </c>
       <c r="B195" s="36" t="s">
-        <v>167</v>
+        <v>144</v>
       </c>
       <c r="D195" s="2" t="s">
         <v>355</v>
       </c>
       <c r="F195" t="s">
-        <v>541</v>
+        <v>518</v>
       </c>
       <c r="G195" s="38" t="s">
-        <v>85</v>
-      </c>
-      <c r="H195" t="s">
-        <v>558</v>
-      </c>
-      <c r="I195" t="s">
-        <v>768</v>
+        <v>584</v>
+      </c>
+      <c r="H195" s="7" t="s">
+        <v>634</v>
       </c>
       <c r="J195">
-        <v>175</v>
-      </c>
-      <c r="K195" t="s">
-        <v>158</v>
+        <v>300</v>
+      </c>
+      <c r="K195" s="5" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="196" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -10427,10 +10468,10 @@
         <v>186</v>
       </c>
       <c r="B196" s="36" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D196" s="2" t="s">
-        <v>108</v>
+        <v>355</v>
       </c>
       <c r="F196" t="s">
         <v>541</v>
@@ -10445,7 +10486,7 @@
         <v>768</v>
       </c>
       <c r="J196">
-        <v>300</v>
+        <v>175</v>
       </c>
       <c r="K196" t="s">
         <v>158</v>
@@ -10453,25 +10494,31 @@
     </row>
     <row r="197" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A197" t="s">
-        <v>81</v>
+        <v>186</v>
       </c>
       <c r="B197" s="36" t="s">
-        <v>206</v>
+        <v>168</v>
+      </c>
+      <c r="D197" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="F197" t="s">
-        <v>518</v>
+        <v>541</v>
       </c>
       <c r="G197" s="38" t="s">
-        <v>584</v>
+        <v>85</v>
       </c>
       <c r="H197" t="s">
-        <v>635</v>
+        <v>558</v>
+      </c>
+      <c r="I197" t="s">
+        <v>768</v>
       </c>
       <c r="J197">
-        <v>-1</v>
-      </c>
-      <c r="K197" s="5" t="s">
-        <v>542</v>
+        <v>300</v>
+      </c>
+      <c r="K197" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="198" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -10479,22 +10526,22 @@
         <v>81</v>
       </c>
       <c r="B198" s="36" t="s">
-        <v>67</v>
+        <v>206</v>
       </c>
       <c r="F198" t="s">
         <v>518</v>
       </c>
       <c r="G198" s="38" t="s">
-        <v>553</v>
+        <v>584</v>
       </c>
       <c r="H198" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="J198">
         <v>-1</v>
       </c>
       <c r="K198" s="5" t="s">
-        <v>66</v>
+        <v>542</v>
       </c>
     </row>
     <row r="199" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -10502,19 +10549,16 @@
         <v>81</v>
       </c>
       <c r="B199" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F199" t="s">
-        <v>703</v>
+        <v>518</v>
       </c>
       <c r="G199" s="38" t="s">
-        <v>85</v>
-      </c>
-      <c r="H199" s="7" t="s">
-        <v>636</v>
-      </c>
-      <c r="I199" t="s">
-        <v>769</v>
+        <v>553</v>
+      </c>
+      <c r="H199" t="s">
+        <v>639</v>
       </c>
       <c r="J199">
         <v>-1</v>
@@ -10528,19 +10572,19 @@
         <v>81</v>
       </c>
       <c r="B200" s="36" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F200" t="s">
         <v>703</v>
       </c>
-      <c r="G200" s="34" t="s">
+      <c r="G200" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="H200" t="s">
-        <v>637</v>
+      <c r="H200" s="7" t="s">
+        <v>636</v>
       </c>
       <c r="I200" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="J200">
         <v>-1</v>
@@ -10554,19 +10598,19 @@
         <v>81</v>
       </c>
       <c r="B201" s="36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F201" t="s">
-        <v>541</v>
-      </c>
-      <c r="G201" s="38" t="s">
+        <v>703</v>
+      </c>
+      <c r="G201" s="34" t="s">
         <v>85</v>
       </c>
       <c r="H201" t="s">
-        <v>560</v>
+        <v>637</v>
       </c>
       <c r="I201" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="J201">
         <v>-1</v>
@@ -10580,7 +10624,7 @@
         <v>81</v>
       </c>
       <c r="B202" s="36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F202" t="s">
         <v>541</v>
@@ -10589,10 +10633,10 @@
         <v>85</v>
       </c>
       <c r="H202" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="I202" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="J202">
         <v>-1</v>
@@ -10603,71 +10647,115 @@
     </row>
     <row r="203" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A203" t="s">
-        <v>357</v>
+        <v>81</v>
       </c>
       <c r="B203" s="36" t="s">
-        <v>148</v>
+        <v>71</v>
       </c>
       <c r="F203" t="s">
-        <v>518</v>
+        <v>541</v>
       </c>
       <c r="G203" s="38" t="s">
-        <v>584</v>
-      </c>
-      <c r="H203" s="7" t="s">
-        <v>634</v>
+        <v>85</v>
+      </c>
+      <c r="H203" t="s">
+        <v>557</v>
+      </c>
+      <c r="I203" t="s">
+        <v>771</v>
       </c>
       <c r="J203">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="K203" s="5" t="s">
-        <v>697</v>
+        <v>66</v>
       </c>
     </row>
     <row r="204" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A204" t="s">
         <v>357</v>
       </c>
-      <c r="B204" s="46" t="s">
-        <v>258</v>
+      <c r="B204" s="36" t="s">
+        <v>148</v>
       </c>
       <c r="F204" t="s">
-        <v>541</v>
+        <v>518</v>
       </c>
       <c r="G204" s="38" t="s">
-        <v>85</v>
-      </c>
-      <c r="H204" t="s">
-        <v>558</v>
-      </c>
-      <c r="I204" t="s">
-        <v>768</v>
+        <v>584</v>
+      </c>
+      <c r="H204" s="7" t="s">
+        <v>634</v>
       </c>
       <c r="J204">
         <v>2</v>
       </c>
       <c r="K204" s="5" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="205" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A205" t="s">
+        <v>357</v>
+      </c>
+      <c r="B205" s="46" t="s">
+        <v>258</v>
+      </c>
+      <c r="F205" t="s">
+        <v>541</v>
+      </c>
+      <c r="G205" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="H205" t="s">
+        <v>558</v>
+      </c>
+      <c r="I205" t="s">
+        <v>768</v>
+      </c>
+      <c r="J205">
+        <v>2</v>
+      </c>
+      <c r="K205" s="5" t="s">
         <v>577</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M204">
-    <sortState ref="A2:M205">
-      <sortCondition ref="A1:A205"/>
+  <autoFilter ref="A1:M205" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState ref="A2:M204">
+      <sortCondition ref="A1:A204"/>
     </sortState>
   </autoFilter>
-  <sortState ref="A2:M205">
-    <sortCondition ref="A2:A205"/>
-    <sortCondition ref="B2:B205"/>
+  <sortState ref="A2:M204">
+    <sortCondition ref="A2:A204"/>
+    <sortCondition ref="B2:B204"/>
   </sortState>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+          <x14:formula1>
+            <xm:f>Sheet1!$A$2:$A$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F205</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
+          <x14:formula1>
+            <xm:f>Sheet1!$B$2:$B$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>G1:G1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
@@ -10719,7 +10807,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="26" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" ht="28" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>401</v>
       </c>
@@ -10772,11 +10860,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFD60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:XFD61"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="125" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32:P32"/>
+    <sheetView topLeftCell="A36" zoomScale="125" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -10812,7 +10900,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>182</v>
       </c>
@@ -10988,7 +11076,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="65" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" ht="70" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -11013,7 +11101,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="65" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" ht="70" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -11091,7 +11179,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="26" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>271</v>
       </c>
@@ -11129,7 +11217,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="39" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:16" ht="42" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>59</v>
       </c>
@@ -11151,7 +11239,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="26" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:16" ht="28" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -11306,7 +11394,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="26" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:16" ht="28" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>339</v>
       </c>
@@ -11429,7 +11517,7 @@
       <c r="L32" s="46"/>
       <c r="P32" s="50"/>
     </row>
-    <row r="33" spans="1:1024 1026:2048 2050:3072 3074:4096 4098:5120 5122:6144 6146:7168 7170:8192 8194:9216 9218:10240 10242:11264 11266:12288 12290:13312 13314:14336 14338:15360 15362:16384" ht="26" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:1024 1026:2048 2050:3072 3074:4096 4098:5120 5122:6144 6146:7168 7170:8192 8194:9216 9218:10240 10242:11264 11266:12288 12290:13312 13314:14336 14338:15360 15362:16384" ht="28" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>401</v>
       </c>
@@ -19831,7 +19919,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="43" spans="1:1024 1026:2048 2050:3072 3074:4096 4098:5120 5122:6144 6146:7168 7170:8192 8194:9216 9218:10240 10242:11264 11266:12288 12290:13312 13314:14336 14338:15360 15362:16384" ht="26" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:1024 1026:2048 2050:3072 3074:4096 4098:5120 5122:6144 6146:7168 7170:8192 8194:9216 9218:10240 10242:11264 11266:12288 12290:13312 13314:14336 14338:15360 15362:16384" ht="28" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>242</v>
       </c>
@@ -19872,7 +19960,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="45" spans="1:1024 1026:2048 2050:3072 3074:4096 4098:5120 5122:6144 6146:7168 7170:8192 8194:9216 9218:10240 10242:11264 11266:12288 12290:13312 13314:14336 14338:15360 15362:16384" ht="39" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:1024 1026:2048 2050:3072 3074:4096 4098:5120 5122:6144 6146:7168 7170:8192 8194:9216 9218:10240 10242:11264 11266:12288 12290:13312 13314:14336 14338:15360 15362:16384" ht="42" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
         <v>242</v>
       </c>
@@ -19894,7 +19982,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="46" spans="1:1024 1026:2048 2050:3072 3074:4096 4098:5120 5122:6144 6146:7168 7170:8192 8194:9216 9218:10240 10242:11264 11266:12288 12290:13312 13314:14336 14338:15360 15362:16384" ht="39" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:1024 1026:2048 2050:3072 3074:4096 4098:5120 5122:6144 6146:7168 7170:8192 8194:9216 9218:10240 10242:11264 11266:12288 12290:13312 13314:14336 14338:15360 15362:16384" ht="42" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
         <v>242</v>
       </c>
@@ -19932,7 +20020,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="48" spans="1:1024 1026:2048 2050:3072 3074:4096 4098:5120 5122:6144 6146:7168 7170:8192 8194:9216 9218:10240 10242:11264 11266:12288 12290:13312 13314:14336 14338:15360 15362:16384" ht="26" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:1024 1026:2048 2050:3072 3074:4096 4098:5120 5122:6144 6146:7168 7170:8192 8194:9216 9218:10240 10242:11264 11266:12288 12290:13312 13314:14336 14338:15360 15362:16384" ht="28" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
         <v>242</v>
       </c>
@@ -20006,46 +20094,52 @@
         <v>643</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
-        <v>243</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="C51" s="2"/>
+        <v>82</v>
+      </c>
+      <c r="B51" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="C51" s="46"/>
       <c r="D51" s="2" t="s">
         <v>196</v>
       </c>
       <c r="E51" t="s">
-        <v>503</v>
-      </c>
-      <c r="F51" t="s">
-        <v>504</v>
+        <v>518</v>
+      </c>
+      <c r="F51" s="38" t="s">
+        <v>584</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>424</v>
-      </c>
-      <c r="H51" s="5" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.15">
+        <v>634</v>
+      </c>
+      <c r="H51" t="s">
+        <v>843</v>
+      </c>
+      <c r="I51">
+        <v>20</v>
+      </c>
+      <c r="J51" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2" t="s">
         <v>196</v>
       </c>
       <c r="E52" t="s">
-        <v>1</v>
+        <v>503</v>
       </c>
       <c r="F52" t="s">
-        <v>2</v>
+        <v>504</v>
       </c>
       <c r="G52" s="7" t="s">
         <v>424</v>
@@ -20054,53 +20148,58 @@
         <v>505</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="91" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>245</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>183</v>
+        <v>246</v>
       </c>
       <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
+      <c r="D53" s="2" t="s">
+        <v>196</v>
+      </c>
       <c r="E53" t="s">
-        <v>541</v>
+        <v>1</v>
       </c>
       <c r="F53" t="s">
-        <v>496</v>
-      </c>
-      <c r="G53" t="s">
-        <v>477</v>
+        <v>2</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>424</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" ht="40" customHeight="1" x14ac:dyDescent="0.15">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="98" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
         <v>51</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>251</v>
+        <v>183</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" t="s">
-        <v>115</v>
+        <v>541</v>
       </c>
       <c r="F54" t="s">
-        <v>33</v>
+        <v>496</v>
+      </c>
+      <c r="G54" t="s">
+        <v>477</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" ht="80" customHeight="1" x14ac:dyDescent="0.15">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
         <v>51</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>204</v>
+        <v>251</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
@@ -20108,124 +20207,143 @@
         <v>115</v>
       </c>
       <c r="F55" t="s">
-        <v>233</v>
+        <v>33</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.15">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="80" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
         <v>51</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>58</v>
+        <v>204</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
       <c r="E56" t="s">
-        <v>498</v>
+        <v>115</v>
       </c>
       <c r="F56" t="s">
-        <v>495</v>
-      </c>
-      <c r="G56" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" ht="39" x14ac:dyDescent="0.15">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
         <v>51</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" t="s">
-        <v>516</v>
+        <v>498</v>
       </c>
       <c r="F57" t="s">
-        <v>376</v>
+        <v>495</v>
       </c>
       <c r="G57" t="s">
-        <v>424</v>
+        <v>230</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" ht="78" x14ac:dyDescent="0.15">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="42" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
         <v>51</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>184</v>
+        <v>8</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" t="s">
-        <v>541</v>
+        <v>516</v>
       </c>
       <c r="F58" t="s">
-        <v>85</v>
+        <v>376</v>
       </c>
       <c r="G58" t="s">
-        <v>452</v>
+        <v>424</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" ht="65" x14ac:dyDescent="0.15">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="84" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
         <v>51</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>52</v>
+        <v>184</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
       <c r="E59" t="s">
-        <v>492</v>
+        <v>541</v>
       </c>
       <c r="F59" t="s">
-        <v>348</v>
+        <v>85</v>
       </c>
       <c r="G59" t="s">
-        <v>260</v>
+        <v>452</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" ht="39" x14ac:dyDescent="0.15">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="70" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
         <v>51</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
       <c r="E60" t="s">
+        <v>492</v>
+      </c>
+      <c r="F60" t="s">
+        <v>348</v>
+      </c>
+      <c r="G60" t="s">
+        <v>260</v>
+      </c>
+      <c r="H60" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="42" x14ac:dyDescent="0.15">
+      <c r="A61" t="s">
+        <v>51</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" t="s">
         <v>349</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F61" t="s">
         <v>422</v>
       </c>
-      <c r="G60" t="s">
+      <c r="G61" t="s">
         <v>257</v>
       </c>
-      <c r="H60" s="5" t="s">
+      <c r="H61" s="5" t="s">
         <v>421</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:XFD1048576">
+  <sortState ref="A2:XFC1048576">
     <sortCondition ref="A3:A1048576"/>
     <sortCondition ref="B3:B1048576"/>
   </sortState>
@@ -20236,7 +20354,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
@@ -20253,7 +20371,7 @@
     <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>494</v>
       </c>
@@ -20279,7 +20397,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>596</v>
       </c>
@@ -20301,7 +20419,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>596</v>
       </c>
@@ -20323,7 +20441,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>596</v>
       </c>
@@ -20345,7 +20463,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>596</v>
       </c>
@@ -20367,7 +20485,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>596</v>
       </c>
@@ -20384,7 +20502,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>596</v>
       </c>
@@ -20401,7 +20519,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>596</v>
       </c>
@@ -20418,7 +20536,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>596</v>
       </c>
@@ -20435,7 +20553,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>596</v>
       </c>
@@ -20452,7 +20570,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>596</v>
       </c>
@@ -20469,7 +20587,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>595</v>
       </c>
@@ -20486,7 +20604,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>595</v>
       </c>
@@ -20503,7 +20621,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>595</v>
       </c>
@@ -20520,7 +20638,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="39" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8" ht="42" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>595</v>
       </c>
@@ -20539,7 +20657,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>595</v>
       </c>
@@ -20561,7 +20679,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>595</v>
       </c>
@@ -20583,7 +20701,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>595</v>
       </c>
@@ -20600,7 +20718,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>595</v>
       </c>
@@ -20617,7 +20735,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>619</v>
       </c>
@@ -20637,7 +20755,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>619</v>
       </c>
@@ -20657,7 +20775,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>619</v>
       </c>
@@ -20677,7 +20795,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>619</v>
       </c>
@@ -20697,7 +20815,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>607</v>
       </c>
@@ -20717,7 +20835,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>607</v>
       </c>
@@ -20737,7 +20855,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>607</v>
       </c>
@@ -20757,7 +20875,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>607</v>
       </c>
@@ -20777,7 +20895,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>578</v>
       </c>
@@ -20796,7 +20914,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>578</v>
       </c>
@@ -20815,7 +20933,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>578</v>
       </c>
@@ -20834,7 +20952,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>82</v>
       </c>
@@ -20860,7 +20978,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>82</v>
       </c>
@@ -20886,7 +21004,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>82</v>
       </c>
@@ -20912,7 +21030,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>82</v>
       </c>
@@ -20938,7 +21056,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>82</v>
       </c>
@@ -20964,7 +21082,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>82</v>
       </c>
@@ -20990,7 +21108,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>82</v>
       </c>
@@ -21016,7 +21134,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>705</v>
       </c>
@@ -21036,7 +21154,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>705</v>
       </c>
@@ -21056,7 +21174,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>705</v>
       </c>
@@ -21076,7 +21194,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>705</v>
       </c>
@@ -21096,7 +21214,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>705</v>
       </c>
@@ -21116,7 +21234,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>705</v>
       </c>
@@ -21136,7 +21254,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
         <v>705</v>
       </c>
@@ -21156,7 +21274,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
         <v>705</v>
       </c>
@@ -21176,7 +21294,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
         <v>705</v>
       </c>
@@ -21196,7 +21314,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
         <v>705</v>
       </c>
@@ -21216,7 +21334,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
         <v>705</v>
       </c>
@@ -21236,7 +21354,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:7" ht="28" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
         <v>705</v>
       </c>
@@ -21256,7 +21374,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:7" ht="28" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
         <v>706</v>
       </c>
@@ -21276,7 +21394,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:7" ht="28" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
         <v>706</v>
       </c>
@@ -21307,11 +21425,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15:G18"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -21324,7 +21442,7 @@
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.5" customWidth="1"/>
-    <col min="9" max="9" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21" customWidth="1"/>
     <col min="10" max="10" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -21370,12 +21488,7 @@
       <c r="B2" s="36" t="s">
         <v>612</v>
       </c>
-      <c r="C2" t="s">
-        <v>616</v>
-      </c>
-      <c r="D2" s="34" t="s">
-        <v>85</v>
-      </c>
+      <c r="D2" s="34"/>
       <c r="E2" t="s">
         <v>84</v>
       </c>
@@ -21397,12 +21510,7 @@
       <c r="B3" s="36" t="s">
         <v>613</v>
       </c>
-      <c r="C3" t="s">
-        <v>616</v>
-      </c>
-      <c r="D3" s="34" t="s">
-        <v>85</v>
-      </c>
+      <c r="D3" s="34"/>
       <c r="E3" t="s">
         <v>84</v>
       </c>
@@ -21424,12 +21532,7 @@
       <c r="B4" s="36" t="s">
         <v>614</v>
       </c>
-      <c r="C4" t="s">
-        <v>616</v>
-      </c>
-      <c r="D4" s="34" t="s">
-        <v>85</v>
-      </c>
+      <c r="D4" s="34"/>
       <c r="E4" t="s">
         <v>84</v>
       </c>
@@ -21451,12 +21554,7 @@
       <c r="B5" s="36" t="s">
         <v>615</v>
       </c>
-      <c r="C5" t="s">
-        <v>616</v>
-      </c>
-      <c r="D5" s="34" t="s">
-        <v>85</v>
-      </c>
+      <c r="D5" s="34"/>
       <c r="E5" t="s">
         <v>84</v>
       </c>
@@ -21746,6 +21844,9 @@
       <c r="G15" s="5" t="s">
         <v>618</v>
       </c>
+      <c r="I15" t="s">
+        <v>853</v>
+      </c>
       <c r="J15" s="43"/>
     </row>
     <row r="16" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -21764,6 +21865,9 @@
       <c r="G16" s="5" t="s">
         <v>618</v>
       </c>
+      <c r="I16" t="s">
+        <v>854</v>
+      </c>
       <c r="J16" s="43"/>
     </row>
     <row r="17" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -21782,6 +21886,9 @@
       <c r="G17" s="5" t="s">
         <v>618</v>
       </c>
+      <c r="I17" t="s">
+        <v>855</v>
+      </c>
       <c r="J17" s="43"/>
     </row>
     <row r="18" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -21799,6 +21906,9 @@
       </c>
       <c r="G18" s="5" t="s">
         <v>618</v>
+      </c>
+      <c r="I18" t="s">
+        <v>856</v>
       </c>
       <c r="J18" s="43"/>
     </row>
@@ -21866,8 +21976,8 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:K21"/>
@@ -21901,7 +22011,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:11" s="24" customFormat="1" ht="79" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" s="24" customFormat="1" ht="85" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="29"/>
       <c r="B4" s="28" t="s">
         <v>72</v>
@@ -22577,8 +22687,8 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:J21"/>
@@ -22611,7 +22721,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:10" s="24" customFormat="1" ht="79" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" s="24" customFormat="1" ht="85" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="29"/>
       <c r="B4" s="28" t="s">
         <v>72</v>
@@ -23213,4 +23323,88 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B1" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>518</v>
+      </c>
+      <c r="B2" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>541</v>
+      </c>
+      <c r="B3" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>848</v>
+      </c>
+      <c r="B4" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>845</v>
+      </c>
+      <c r="B5" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>846</v>
+      </c>
+      <c r="B6" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>